<commit_message>
:zap: UPDATE - new documentation + plugin improvements
</commit_message>
<xml_diff>
--- a/test-cases/Ecard TC_ENG/eCard_test cards.xlsx
+++ b/test-cases/Ecard TC_ENG/eCard_test cards.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7454B7E1-325A-4028-94FE-5BEBEE5F8EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{78535F17-0284-4CF2-A28B-0E0D917095D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="eCard_testovacie karty" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>VISA 1</t>
   </si>
@@ -55,12 +55,18 @@
   <si>
     <t>Mastercard 1</t>
   </si>
+  <si>
+    <t>5892290000424181</t>
+  </si>
+  <si>
+    <t>4595980021202763</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +123,13 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -312,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -336,12 +349,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -354,10 +361,32 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -368,18 +397,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -399,9 +416,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -439,9 +456,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -474,26 +491,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -526,26 +526,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -719,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F20"/>
+  <dimension ref="B1:O20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -733,133 +716,135 @@
     <col min="4" max="4" width="14.1796875" style="2" customWidth="1"/>
     <col min="5" max="5" width="18.54296875" style="1" customWidth="1"/>
     <col min="6" max="6" width="25.54296875" customWidth="1"/>
+    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
     </row>
-    <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="17" t="s">
+    <row r="2" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19"/>
-    </row>
-    <row r="3" spans="2:6" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="11" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="24"/>
+    </row>
+    <row r="3" spans="2:15" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="15">
-        <v>4595980021202760</v>
-      </c>
-      <c r="C4" s="20" t="s">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B4" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="15">
         <v>45657</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="16">
-        <v>5892290000424180</v>
-      </c>
-      <c r="C5" s="21" t="s">
+    <row r="5" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="17">
         <v>45657</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="7"/>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="7"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7"/>
       <c r="E8" s="8"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="6"/>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B11" s="19"/>
       <c r="C11" s="6"/>
       <c r="D11" s="7"/>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="7"/>
       <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="O12" s="19"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="7"/>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="7"/>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C15" s="6"/>
       <c r="D15" s="7"/>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="7"/>
       <c r="E16" s="8"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="21"/>
       <c r="D17" s="7"/>
       <c r="E17" s="8"/>
     </row>
@@ -887,5 +872,8 @@
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B4:B5" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
:memo: TEST DATA - added new test data
</commit_message>
<xml_diff>
--- a/test-cases/Ecard TC_ENG/eCard_test cards.xlsx
+++ b/test-cases/Ecard TC_ENG/eCard_test cards.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78535F17-0284-4CF2-A28B-0E0D917095D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40BB8BB-DFEB-4B87-B347-E9D10C345B70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,17 +56,17 @@
     <t>Mastercard 1</t>
   </si>
   <si>
+    <t>4595980021202763</t>
+  </si>
+  <si>
     <t>5892290000424181</t>
-  </si>
-  <si>
-    <t>4595980021202763</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,13 +123,6 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -325,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -349,6 +342,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -361,32 +360,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -397,6 +380,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -702,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:O20"/>
+  <dimension ref="B1:F20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -716,135 +705,133 @@
     <col min="4" max="4" width="14.1796875" style="2" customWidth="1"/>
     <col min="5" max="5" width="18.54296875" style="1" customWidth="1"/>
     <col min="6" max="6" width="25.54296875" customWidth="1"/>
-    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
     </row>
-    <row r="2" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="22" t="s">
+    <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="24"/>
-    </row>
-    <row r="3" spans="2:15" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="9" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="21"/>
+    </row>
+    <row r="3" spans="2:6" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B4" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="14" t="s">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B4" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="15">
-        <v>45657</v>
+      <c r="D4" s="17">
+        <v>47118</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="13" t="s">
-        <v>9</v>
+    <row r="5" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="17">
-        <v>45657</v>
+      <c r="D5" s="18">
+        <v>47118</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="7"/>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="7"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7"/>
       <c r="E8" s="8"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B11" s="19"/>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="7"/>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="7"/>
       <c r="E12" s="8"/>
-      <c r="O12" s="19"/>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="7"/>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="7"/>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C15" s="6"/>
       <c r="D15" s="7"/>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="7"/>
       <c r="E16" s="8"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B17" s="20"/>
-      <c r="C17" s="21"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
       <c r="D17" s="7"/>
       <c r="E17" s="8"/>
     </row>
@@ -872,8 +859,11 @@
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="B4:B5" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{db32df23-4916-48f4-a56e-809ab3c7f628}" enabled="1" method="Standard" siteId="{b637e391-2c95-40cc-bc29-99bcff6cf683}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>